<commit_message>
Historique des entrainements - ajouter un tableau sur le nombre total de sauts réalisés sur la période sélectionnée
</commit_message>
<xml_diff>
--- a/TODO_app_synergy.xlsx
+++ b/TODO_app_synergy.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>TODO et questions</t>
   </si>
@@ -52,6 +52,9 @@
     <t>visualisation entrainement - changer "Timeline de l'entrainement" par "Sauts pedant l'entrainement"</t>
   </si>
   <si>
+    <t>visualisation entrainement - Modifier l’ordre et les labels dans le tableau</t>
+  </si>
+  <si>
     <t>Historique des entrainements - choisir la période [dernière semaine | dernier mois | ...]</t>
   </si>
   <si>
@@ -61,6 +64,9 @@
     <t>Historique des entrainements - utiliser un dégradé complet entre rouge et vert</t>
   </si>
   <si>
+    <t>En cours, pas convaincu...</t>
+  </si>
+  <si>
     <t>Historique des entrainements - ajouter l'évoluation de chacun des paramètres (menu déroulant) mois par mois en choisissant la profondeur de l'historique (2 à 24 mois par exemple, avec un slider) - médiane et interquartile - choix du saut (type et nombre de rotation)</t>
   </si>
   <si>
@@ -73,10 +79,16 @@
     <t>Comparer athlètes - ajouter la période (3,6, 12, 24 mois)</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>Comparer athlètes - remplacer "Total de sauts" - "Nombre de sauts"</t>
   </si>
   <si>
     <t>Comparer athlètes - c'est quoi "saut par entrainement" - donner plutôt la fréqeuence (saut/min)</t>
+  </si>
+  <si>
+    <t>A voir</t>
   </si>
   <si>
     <t>Comparer athlètes - remplacer "durée du saut" par "temps de vol"</t>
@@ -139,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -161,6 +173,12 @@
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general" wrapText="1"/>
@@ -473,16 +491,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="61.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="7.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="8.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="10" width="54.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="10" width="61.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="11" width="7.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="11" width="8.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="12" width="54.57642857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -563,7 +581,9 @@
       <c r="C6" s="5">
         <v>2</v>
       </c>
-      <c r="D6" s="6"/>
+      <c r="D6" s="6" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="27">
       <c r="A7" s="4" t="s">
@@ -580,16 +600,18 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="27">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="5">
-        <v>2</v>
-      </c>
-      <c r="C8" s="5">
-        <v>2</v>
-      </c>
-      <c r="D8" s="6"/>
+      <c r="B8" s="7">
+        <v>2</v>
+      </c>
+      <c r="C8" s="7">
+        <v>1</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="27">
       <c r="A9" s="4" t="s">
@@ -599,64 +621,72 @@
         <v>2</v>
       </c>
       <c r="C9" s="5">
-        <v>1</v>
-      </c>
-      <c r="D9" s="6"/>
+        <v>2</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="27">
       <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" s="5">
-        <v>2</v>
-      </c>
-      <c r="D10" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="48">
+        <v>1</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="27">
       <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11" s="5">
+        <v>2</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="48">
+      <c r="A12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="5">
+        <v>2</v>
+      </c>
+      <c r="C12" s="5">
         <v>3</v>
       </c>
-      <c r="D11" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="27">
-      <c r="A12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="5">
-        <v>3</v>
-      </c>
-      <c r="C12" s="5">
-        <v>1</v>
-      </c>
       <c r="D12" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="27">
       <c r="A13" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B13" s="5">
         <v>3</v>
       </c>
       <c r="C13" s="5">
-        <v>2</v>
-      </c>
-      <c r="D13" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="16.5">
       <c r="A14" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C14" s="5">
         <v>2</v>
@@ -665,51 +695,71 @@
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="16.5">
       <c r="A15" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B15" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" s="5">
-        <v>1</v>
-      </c>
-      <c r="D15" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="27">
+        <v>2</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="16.5">
       <c r="A16" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B16" s="5">
         <v>2</v>
       </c>
       <c r="C16" s="5">
-        <v>2</v>
-      </c>
-      <c r="D16" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="16.5">
+        <v>1</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="32.25">
       <c r="A17" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B17" s="5">
         <v>2</v>
       </c>
       <c r="C17" s="5">
-        <v>1</v>
-      </c>
-      <c r="D17" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="16.5">
+        <v>2</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
       <c r="A18" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B18" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18" s="5">
+        <v>1</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="36.75">
+      <c r="A19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="5">
+        <v>1</v>
+      </c>
+      <c r="C19" s="5">
         <v>3</v>
       </c>
-      <c r="D18" s="6"/>
+      <c r="D19" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>